<commit_message>
- LM74670 ideal diode breakout board
</commit_message>
<xml_diff>
--- a/ORG1510-MK4 breakout.xlsx
+++ b/ORG1510-MK4 breakout.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
   <si>
     <t>Part</t>
   </si>
@@ -89,13 +89,19 @@
   </si>
   <si>
     <t>MOUSER URL</t>
+  </si>
+  <si>
+    <t>https://hr.mouser.com/ProductDetail/Microsemi/SMBJ4729Ae3-TR13/?qs=%2fha2pyFadugozOLVQX8oU%252bLu9j3Llt5qc4Sq4QXvUCgpmf6R2dENSw%3d%3d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">494-SMBJ4729AE3/TR13 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -249,8 +255,17 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -428,6 +443,18 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -547,7 +574,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -590,14 +617,24 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -631,6 +668,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -941,7 +979,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -952,7 +990,8 @@
     <col min="4" max="4" width="14.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="8.88671875" style="1"/>
   </cols>
@@ -984,10 +1023,13 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2">
         <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -1001,10 +1043,13 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2">
         <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -1018,11 +1063,14 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>12</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>7</v>
@@ -1035,10 +1083,13 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2">
         <v>6</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -1052,11 +1103,14 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>15</v>
+      </c>
+      <c r="C6" s="3">
+        <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>16</v>
@@ -1067,13 +1121,22 @@
       <c r="F6" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="G6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>20</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>20</v>
@@ -1083,6 +1146,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H6" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>